<commit_message>
Listeners classes Data provider and tree,Graph,datastructure code added
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/SignInDetailsExcel.xlsx
+++ b/src/test/resources/testData/SignInDetailsExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sride\eclipse-workspace\DsAlgo_TestNG\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E34A7D-2620-465A-9BE0-4C82AED99ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46642801-65D1-4EE8-B380-203A9740705C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8928" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignInDetails" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>Username</t>
   </si>
@@ -105,13 +105,22 @@
   </si>
   <si>
     <t>print "hello"</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>alert window with error will come</t>
+  </si>
+  <si>
+    <t>Expected Output</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +138,27 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -152,8 +182,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -1462,7 +1495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37BD0272-DA0E-4B78-9A3B-F8EE4F847E97}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1606,31 +1639,49 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="39.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>24</v>
+      <c r="B3" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated code with reports added
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/SignInDetailsExcel.xlsx
+++ b/src/test/resources/testData/SignInDetailsExcel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TESTNG\DsAlgo_TestNg\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sride\eclipse-workspace\DsAlgo_TestNG\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB46B1C-2344-4FC4-A553-59B3B4E4C957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A7092B-63A1-4718-A0FE-9BC681BEA80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignInDetails" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="TryEditor" sheetId="3" r:id="rId4"/>
     <sheet name="LoginInvalid" sheetId="7" r:id="rId5"/>
     <sheet name="Array Questions" sheetId="4" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -1693,7 +1692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB65D1E-A991-4C85-BF70-7A4EF8802171}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
@@ -1749,7 +1748,7 @@
   </sheetPr>
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1771,18 +1770,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74496FB-AD36-4BD4-B220-00B3B0ACEAD9}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>